<commit_message>
Changes hvor jeg ikke har gjort noget
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Scen_GRD_Constraints.xlsx
+++ b/TIMES-DE/SuppXLS/Scen_GRD_Constraints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES_AZ\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFA2BA8-8D12-4DEA-814A-5A158FB0C767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83E5F65-7D56-FC46-8AA6-71605F987B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="624" windowWidth="20280" windowHeight="16212" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="20280" windowHeight="15540" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="33" r:id="rId1"/>
@@ -135,15 +135,6 @@
     <t>Mikkel Bosack Simonsen</t>
   </si>
   <si>
-    <t>AZ1</t>
-  </si>
-  <si>
-    <t>AZ2</t>
-  </si>
-  <si>
-    <t>AZ3</t>
-  </si>
-  <si>
     <t>FT-GRDHET*</t>
   </si>
   <si>
@@ -170,6 +161,15 @@
   <si>
     <t>Existing and new Transmissions lines</t>
   </si>
+  <si>
+    <t>DE1</t>
+  </si>
+  <si>
+    <t>DE2</t>
+  </si>
+  <si>
+    <t>DE3</t>
+  </si>
 </sst>
 </file>
 
@@ -180,12 +180,12 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="#,##0;\-\ #,##0;_-\ &quot;- &quot;"/>
-    <numFmt numFmtId="172" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
-    <numFmt numFmtId="173" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="175" formatCode="0.0%"/>
-    <numFmt numFmtId="176" formatCode="#,##0;#\ ##0"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="#,##0;\-\ #,##0;_-\ &quot;- &quot;"/>
+    <numFmt numFmtId="170" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
+    <numFmt numFmtId="171" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="173" formatCode="#,##0;#\ ##0"/>
   </numFmts>
   <fonts count="77">
     <font>
@@ -1412,273 +1412,273 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -2364,270 +2364,270 @@
     <xf numFmtId="0" fontId="6" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -3477,7 +3477,7 @@
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="65" fillId="0" borderId="0">
+    <xf numFmtId="172" fontId="65" fillId="0" borderId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="66" fillId="0" borderId="0">
@@ -3577,7 +3577,7 @@
     <xf numFmtId="0" fontId="72" fillId="0" borderId="25" applyNumberFormat="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="73" fillId="0" borderId="25">
+    <xf numFmtId="173" fontId="73" fillId="0" borderId="25">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3598,94 +3598,94 @@
     <xf numFmtId="0" fontId="55" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="55" fillId="54" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="55" fillId="58" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="52" fillId="33" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="55" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3975,94 +3975,94 @@
     <xf numFmtId="0" fontId="3" fillId="34" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7823,14 +7823,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="21" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="21" customWidth="1"/>
     <col min="5" max="5" width="60.33203125" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="21"/>
+    <col min="6" max="16384" width="9.1640625" style="21"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5">
@@ -7880,63 +7880,63 @@
   </sheetPr>
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="25"/>
+    <col min="1" max="1" width="9.1640625" style="25"/>
     <col min="2" max="2" width="24" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="138.44140625" style="25" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="25"/>
+    <col min="3" max="3" width="138.5" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18">
+    <row r="1" spans="2:3" ht="19">
       <c r="B1" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="14.4">
+    <row r="3" spans="2:3" ht="15">
       <c r="B3" s="26" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="14.4">
+    <row r="4" spans="2:3" ht="15">
       <c r="B4" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="14.4">
+    <row r="5" spans="2:3" ht="15">
       <c r="B5" s="26"/>
     </row>
-    <row r="6" spans="2:3" ht="14.4">
+    <row r="6" spans="2:3" ht="15">
       <c r="B6" s="26"/>
     </row>
-    <row r="7" spans="2:3" ht="14.4">
+    <row r="7" spans="2:3" ht="15">
       <c r="B7" s="26"/>
     </row>
-    <row r="8" spans="2:3" ht="14.4">
+    <row r="8" spans="2:3" ht="15">
       <c r="B8" s="26"/>
     </row>
-    <row r="9" spans="2:3" ht="14.4">
+    <row r="9" spans="2:3" ht="15">
       <c r="B9" s="26"/>
     </row>
-    <row r="10" spans="2:3" ht="14.4">
+    <row r="10" spans="2:3" ht="15">
       <c r="B10" s="26"/>
     </row>
-    <row r="11" spans="2:3" ht="14.4">
+    <row r="11" spans="2:3" ht="15">
       <c r="B11" s="27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="14.4">
+    <row r="12" spans="2:3" ht="15">
       <c r="B12" s="26"/>
     </row>
-    <row r="13" spans="2:3" ht="14.4">
+    <row r="13" spans="2:3" ht="15">
       <c r="B13" s="28" t="s">
         <v>19</v>
       </c>
@@ -7965,20 +7965,20 @@
   </sheetPr>
   <dimension ref="B1:M29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
     <col min="2" max="2" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.109375" style="1"/>
+    <col min="3" max="4" width="9.1640625" style="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
     <col min="7" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="9" max="9" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
@@ -7993,7 +7993,7 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="2:13" ht="15" thickBot="1">
+    <row r="5" spans="2:13" ht="16" thickBot="1">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -8007,20 +8007,20 @@
         <v>4</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="2:13" ht="15" thickBot="1">
+    <row r="6" spans="2:13" ht="16" thickBot="1">
       <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
@@ -8045,7 +8045,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1">
         <v>2010</v>
@@ -8062,7 +8062,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J7" s="11"/>
     </row>
@@ -8071,7 +8071,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1">
         <v>2012</v>
@@ -8088,7 +8088,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J8" s="11"/>
     </row>
@@ -8097,7 +8097,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1">
         <v>2020</v>
@@ -8114,7 +8114,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -8123,7 +8123,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" s="9">
         <v>2030</v>
@@ -8140,7 +8140,7 @@
         <v>222.3</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -8149,7 +8149,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" s="3">
         <v>2050</v>
@@ -8167,10 +8167,10 @@
         <v>444.6</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M11" s="33"/>
     </row>
@@ -8180,25 +8180,25 @@
         <v>8</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="9">
         <v>2010</v>
       </c>
       <c r="F12" s="18">
-        <f>F7/2</f>
+        <f t="shared" ref="F12:H14" si="0">F7/2</f>
         <v>5</v>
       </c>
       <c r="G12" s="18">
-        <f>G7/2</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="H12" s="18">
-        <f>H7/2</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -8207,25 +8207,25 @@
         <v>8</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" s="9">
         <v>2012</v>
       </c>
       <c r="F13" s="18">
-        <f>F8/2</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G13" s="18">
-        <f>G8/2</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="H13" s="18">
-        <f>H8/2</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -8234,25 +8234,25 @@
         <v>8</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" s="9">
         <v>2020</v>
       </c>
       <c r="F14" s="18">
-        <f>F9/2</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G14" s="18">
-        <f>G9/2</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="H14" s="18">
-        <f>H9/2</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -8261,25 +8261,25 @@
         <v>8</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="9">
         <v>2030</v>
       </c>
       <c r="F15" s="18">
-        <f t="shared" ref="F15:H16" si="0">F10/2</f>
+        <f t="shared" ref="F15:H16" si="1">F10/2</f>
         <v>1111.5</v>
       </c>
       <c r="G15" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>111.15</v>
       </c>
       <c r="H15" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>111.15</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -8288,28 +8288,28 @@
         <v>8</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3">
         <v>2040</v>
       </c>
       <c r="F16" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2223</v>
       </c>
       <c r="G16" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>222.3</v>
       </c>
       <c r="H16" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>222.3</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:12">
@@ -8336,7 +8336,7 @@
         <v>0.25</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:12">
@@ -8351,19 +8351,19 @@
         <v>2012</v>
       </c>
       <c r="F18" s="18">
-        <f t="shared" ref="F18:H18" si="1">F13/2</f>
+        <f t="shared" ref="F18:H18" si="2">F13/2</f>
         <v>2.5</v>
       </c>
       <c r="G18" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="H18" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:12">
@@ -8377,19 +8377,19 @@
         <v>2020</v>
       </c>
       <c r="F19" s="18">
-        <f t="shared" ref="F19:H19" si="2">F14/2</f>
+        <f t="shared" ref="F19:H19" si="3">F14/2</f>
         <v>2.5</v>
       </c>
       <c r="G19" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="H19" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="I19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:12">
@@ -8403,22 +8403,22 @@
         <v>2030</v>
       </c>
       <c r="F20" s="18">
-        <f t="shared" ref="F20:H20" si="3">F15/2</f>
+        <f t="shared" ref="F20:H20" si="4">F15/2</f>
         <v>555.75</v>
       </c>
       <c r="G20" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55.575000000000003</v>
       </c>
       <c r="H20" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55.575000000000003</v>
       </c>
       <c r="I20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15" thickBot="1">
+    <row r="21" spans="2:12" ht="16" thickBot="1">
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
@@ -8429,22 +8429,22 @@
         <v>2040</v>
       </c>
       <c r="F21" s="18">
-        <f t="shared" ref="F21:H21" si="4">F16/2</f>
+        <f t="shared" ref="F21:H21" si="5">F16/2</f>
         <v>1111.5</v>
       </c>
       <c r="G21" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>111.15</v>
       </c>
       <c r="H21" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>111.15</v>
       </c>
       <c r="I21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L21" s="33" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -8468,7 +8468,7 @@
         <v>5</v>
       </c>
       <c r="I22" s="32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="2:12">
@@ -8488,6 +8488,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -8710,15 +8719,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -8726,13 +8726,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6B9E7C2-787E-4D9C-B562-594058D54B6C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29708D-970D-48DD-9E4A-5A0CFA626223}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29708D-970D-48DD-9E4A-5A0CFA626223}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6B9E7C2-787E-4D9C-B562-594058D54B6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
+    <ds:schemaRef ds:uri="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3BDCBCB-54F4-4172-B29B-BA4C04015FBC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3BDCBCB-54F4-4172-B29B-BA4C04015FBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update af faste scenarie filer
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Scen_GRD_Constraints.xlsx
+++ b/TIMES-DE/SuppXLS/Scen_GRD_Constraints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julius Steensberg\OneDrive\Desktop\GitHub\Bachelor_Git\TIMES-DE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83E5F65-7D56-FC46-8AA6-71605F987B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F4AA1E-A60C-4A6D-88C6-8D7243D62B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="20280" windowHeight="15540" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="33" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -170,6 +170,12 @@
   <si>
     <t>DE3</t>
   </si>
+  <si>
+    <t>DE4</t>
+  </si>
+  <si>
+    <t>DE5</t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +193,7 @@
     <numFmt numFmtId="172" formatCode="0.0%"/>
     <numFmt numFmtId="173" formatCode="#,##0;#\ ##0"/>
   </numFmts>
-  <fonts count="77">
+  <fonts count="78">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -686,6 +692,10 @@
       <color indexed="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="63">
@@ -4406,6 +4416,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2864">
+    <cellStyle name="20 % - Farve1" xfId="1701" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve2" xfId="1705" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve3" xfId="1709" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve4" xfId="1713" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve5" xfId="1717" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Farve6" xfId="1721" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20 % - Markeringsfarve1" xfId="2193" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="20 % - Markeringsfarve1 2" xfId="2010" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20 % - Markeringsfarve1 2 2" xfId="2011" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -4442,17 +4458,11 @@
     <cellStyle name="20 % - Markeringsfarve6 3" xfId="2037" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="20 % - Markeringsfarve6 4" xfId="2038" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
     <cellStyle name="20 % - Markeringsfarve6 5" xfId="2039" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="20% - Accent1" xfId="1701" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="2040" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="20% - Accent2" xfId="1705" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent2 2" xfId="2041" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="20% - Accent3" xfId="1709" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20% - Accent3 2" xfId="2042" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="20% - Accent4" xfId="1713" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20% - Accent4 2" xfId="2043" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="20% - Accent5" xfId="1717" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20% - Accent5 2" xfId="2044" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="20% - Accent6" xfId="1721" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20% - Accent6 2" xfId="2045" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
     <cellStyle name="20% - Colore 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
     <cellStyle name="20% - Colore 1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
@@ -4466,6 +4476,12 @@
     <cellStyle name="20% - Colore 5 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
     <cellStyle name="20% - Colore 6" xfId="11" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
     <cellStyle name="20% - Colore 6 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="40 % - Farve1" xfId="1702" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve2" xfId="1706" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve3" xfId="1710" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve4" xfId="1714" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve5" xfId="1718" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Farve6" xfId="1722" builtinId="51" customBuiltin="1"/>
     <cellStyle name="40 % - Markeringsfarve1" xfId="2199" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
     <cellStyle name="40 % - Markeringsfarve1 2" xfId="2046" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
     <cellStyle name="40 % - Markeringsfarve1 2 2" xfId="2047" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
@@ -4502,17 +4518,11 @@
     <cellStyle name="40 % - Markeringsfarve6 3" xfId="2073" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
     <cellStyle name="40 % - Markeringsfarve6 4" xfId="2074" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
     <cellStyle name="40 % - Markeringsfarve6 5" xfId="2075" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="40% - Accent1" xfId="1702" builtinId="31" customBuiltin="1"/>
     <cellStyle name="40% - Accent1 2" xfId="2076" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="40% - Accent2" xfId="1706" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40% - Accent2 2" xfId="2077" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="40% - Accent3" xfId="1710" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40% - Accent3 2" xfId="2078" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="40% - Accent4" xfId="1714" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent4 2" xfId="2079" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="40% - Accent5" xfId="1718" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent5 2" xfId="2080" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="40% - Accent6" xfId="1722" builtinId="51" customBuiltin="1"/>
     <cellStyle name="40% - Accent6 2" xfId="2081" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
     <cellStyle name="40% - Colore 1" xfId="13" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
     <cellStyle name="40% - Colore 1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
@@ -4527,23 +4537,23 @@
     <cellStyle name="40% - Colore 6" xfId="23" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
     <cellStyle name="40% - Colore 6 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
     <cellStyle name="5x indented GHG Textfiels" xfId="25" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="60 % - Farve1" xfId="1703" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve2" xfId="1707" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve3" xfId="1711" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve4" xfId="1715" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve5" xfId="1719" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Farve6" xfId="1723" builtinId="52" customBuiltin="1"/>
     <cellStyle name="60 % - Markeringsfarve1" xfId="2205" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
     <cellStyle name="60 % - Markeringsfarve2" xfId="2206" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
     <cellStyle name="60 % - Markeringsfarve3" xfId="2207" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
     <cellStyle name="60 % - Markeringsfarve4" xfId="2208" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
     <cellStyle name="60 % - Markeringsfarve5" xfId="2209" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
     <cellStyle name="60 % - Markeringsfarve6" xfId="2210" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="60% - Accent1" xfId="1703" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent1 2" xfId="2082" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="60% - Accent2" xfId="1707" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent2 2" xfId="2083" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="60% - Accent3" xfId="1711" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60% - Accent3 2" xfId="2084" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="60% - Accent4" xfId="1715" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Accent4 2" xfId="2085" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="60% - Accent5" xfId="1719" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Accent5 2" xfId="2086" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="60% - Accent6" xfId="1723" builtinId="52" customBuiltin="1"/>
     <cellStyle name="60% - Accent6 2" xfId="2087" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
     <cellStyle name="60% - Colore 1" xfId="26" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
     <cellStyle name="60% - Colore 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
@@ -4551,21 +4561,15 @@
     <cellStyle name="60% - Colore 4" xfId="29" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
     <cellStyle name="60% - Colore 5" xfId="30" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
     <cellStyle name="60% - Colore 6" xfId="31" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Accent1" xfId="1700" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 2" xfId="2088" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Accent2" xfId="1704" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 2" xfId="2089" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Accent3" xfId="1708" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 2" xfId="2090" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Accent4" xfId="1712" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 2" xfId="2091" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Accent5" xfId="1716" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 2" xfId="2092" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Accent6" xfId="1720" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 2" xfId="2093" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Advarselstekst" xfId="1697" builtinId="11" customBuiltin="1"/>
     <cellStyle name="AggOrange_CRFReport-template" xfId="32" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
     <cellStyle name="AggOrange9_CRFReport-template" xfId="33" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="Bad" xfId="1690" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Bad 2" xfId="34" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
     <cellStyle name="Bad 2 2" xfId="2094" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
     <cellStyle name="Bad 3" xfId="35" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
@@ -4575,6 +4579,7 @@
     <cellStyle name="Bemærk! 3 2" xfId="2098" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
     <cellStyle name="Bemærk! 4" xfId="2099" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
     <cellStyle name="Bemærk! 5" xfId="2100" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Beregning" xfId="1694" builtinId="22" customBuiltin="1"/>
     <cellStyle name="C01_Main head" xfId="2101" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
     <cellStyle name="C02_Column heads" xfId="2102" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
     <cellStyle name="C03_Sub head bold" xfId="2103" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
@@ -4596,12 +4601,10 @@
     <cellStyle name="Calcolo 4" xfId="1728" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
     <cellStyle name="Calcolo 5" xfId="1729" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
     <cellStyle name="Calcolo 6" xfId="1730" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="Calculation" xfId="1694" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Calculation 2" xfId="39" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
     <cellStyle name="Calculation 2 2" xfId="2112" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
     <cellStyle name="Cella collegata" xfId="40" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
     <cellStyle name="Cella da controllare" xfId="41" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="Check Cell" xfId="1696" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Check Cell 2" xfId="2113" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
     <cellStyle name="Colore 1" xfId="42" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
     <cellStyle name="Colore 2" xfId="43" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
@@ -5000,18 +5003,20 @@
     <cellStyle name="Euro 9 4" xfId="329" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
     <cellStyle name="Euro 9 4 2" xfId="2297" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
     <cellStyle name="Euro 9 5" xfId="2298" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
-    <cellStyle name="Explanatory Text" xfId="1698" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Explanatory Text 2" xfId="2130" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Farve1" xfId="1700" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Farve2" xfId="1704" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Farve3" xfId="1708" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Farve4" xfId="1712" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Farve5" xfId="1716" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Farve6" xfId="1720" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Fixed2 - Type2" xfId="330" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
-    <cellStyle name="Good" xfId="1689" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Forklarende tekst" xfId="1698" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="God" xfId="1689" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Good 2" xfId="2131" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
-    <cellStyle name="Heading 1" xfId="1685" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="2132" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
-    <cellStyle name="Heading 2" xfId="1686" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 2 2" xfId="2133" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
-    <cellStyle name="Heading 3" xfId="1687" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 3 2" xfId="2134" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
-    <cellStyle name="Heading 4" xfId="1688" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Heading 4 2" xfId="2135" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
     <cellStyle name="Hyperlink 2" xfId="2009" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
     <cellStyle name="Hyperlink 3" xfId="2136" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
@@ -5043,8 +5048,8 @@
     <cellStyle name="Komma 8" xfId="2148" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
     <cellStyle name="Komma 9" xfId="2149" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
     <cellStyle name="Kontroller celle" xfId="2300" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Kontrollér celle" xfId="1696" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Link 2" xfId="2150" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
-    <cellStyle name="Linked Cell" xfId="1695" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Linked Cell 2" xfId="2151" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
     <cellStyle name="Markeringsfarve1" xfId="2301" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
     <cellStyle name="Markeringsfarve2" xfId="2302" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
@@ -6639,6 +6644,10 @@
     <cellStyle name="Output 2 6" xfId="1997" xr:uid="{00000000-0005-0000-0000-0000B6080000}"/>
     <cellStyle name="Output 3" xfId="1272" xr:uid="{00000000-0005-0000-0000-0000B7080000}"/>
     <cellStyle name="Output 3 2" xfId="2676" xr:uid="{00000000-0005-0000-0000-0000B8080000}"/>
+    <cellStyle name="Overskrift 1" xfId="1685" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Overskrift 2" xfId="1686" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Overskrift 3" xfId="1687" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Overskrift 4" xfId="1688" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Percen - Type1" xfId="1273" xr:uid="{00000000-0005-0000-0000-0000B9080000}"/>
     <cellStyle name="Percent 2" xfId="1274" xr:uid="{00000000-0005-0000-0000-0000BA080000}"/>
     <cellStyle name="Percent 2 2" xfId="1275" xr:uid="{00000000-0005-0000-0000-0000BB080000}"/>
@@ -7180,6 +7189,7 @@
     <cellStyle name="Procent 5 2" xfId="2181" xr:uid="{00000000-0005-0000-0000-0000D30A0000}"/>
     <cellStyle name="Procent 6" xfId="2182" xr:uid="{00000000-0005-0000-0000-0000D40A0000}"/>
     <cellStyle name="Procent 7" xfId="2183" xr:uid="{00000000-0005-0000-0000-0000D50A0000}"/>
+    <cellStyle name="Sammenkædet celle" xfId="1695" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Standard_Sce_D_Extraction" xfId="1668" xr:uid="{00000000-0005-0000-0000-0000D60A0000}"/>
     <cellStyle name="Style 134 2" xfId="2184" xr:uid="{00000000-0005-0000-0000-0000D70A0000}"/>
     <cellStyle name="Style 140" xfId="2185" xr:uid="{00000000-0005-0000-0000-0000D80A0000}"/>
@@ -7263,9 +7273,9 @@
     <cellStyle name="Totale 4" xfId="2004" xr:uid="{00000000-0005-0000-0000-0000260B0000}"/>
     <cellStyle name="Totale 5" xfId="2005" xr:uid="{00000000-0005-0000-0000-0000270B0000}"/>
     <cellStyle name="Totale 6" xfId="2006" xr:uid="{00000000-0005-0000-0000-0000280B0000}"/>
+    <cellStyle name="Ugyldig" xfId="1690" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Valore non valido" xfId="1682" xr:uid="{00000000-0005-0000-0000-0000290B0000}"/>
     <cellStyle name="Valore valido" xfId="1683" xr:uid="{00000000-0005-0000-0000-00002A0B0000}"/>
-    <cellStyle name="Warning Text" xfId="1697" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Warning Text 2" xfId="2190" xr:uid="{00000000-0005-0000-0000-00002C0B0000}"/>
     <cellStyle name="X08_Total Oil" xfId="2191" xr:uid="{00000000-0005-0000-0000-00002D0B0000}"/>
     <cellStyle name="X12_Total Figs 1 dec" xfId="2192" xr:uid="{00000000-0005-0000-0000-00002E0B0000}"/>
@@ -7309,134 +7319,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="IEA Data"/>
-      <sheetName val="E&amp;D Drivers"/>
       <sheetName val="AGR_Fuels"/>
-      <sheetName val="AGR"/>
-      <sheetName val="RES_Fuels"/>
-      <sheetName val="RH1"/>
-      <sheetName val="RH2"/>
-      <sheetName val="RH3"/>
-      <sheetName val="RH4"/>
-      <sheetName val="RC1"/>
-      <sheetName val="RC2"/>
-      <sheetName val="RC3"/>
-      <sheetName val="RC4"/>
-      <sheetName val="RHW"/>
-      <sheetName val="RRF"/>
-      <sheetName val="RCW"/>
-      <sheetName val="RCD"/>
-      <sheetName val="RK1"/>
-      <sheetName val="RK2"/>
-      <sheetName val="RK3"/>
-      <sheetName val="RK4"/>
-      <sheetName val="RDW"/>
-      <sheetName val="RME"/>
-      <sheetName val="RL1"/>
-      <sheetName val="RL2"/>
-      <sheetName val="RL3"/>
-      <sheetName val="RL4"/>
-      <sheetName val="COM_Fuels"/>
-      <sheetName val="CH1"/>
-      <sheetName val="CH2"/>
-      <sheetName val="CH3"/>
-      <sheetName val="CH4"/>
-      <sheetName val="CC1"/>
-      <sheetName val="CC2"/>
-      <sheetName val="CC3"/>
-      <sheetName val="CC4"/>
-      <sheetName val="CHW"/>
-      <sheetName val="CAA"/>
-      <sheetName val="CLA"/>
-      <sheetName val="ElastPar"/>
-      <sheetName val="Conversion Factors"/>
-      <sheetName val="Intro"/>
-      <sheetName val="TechRep"/>
-      <sheetName val="Other_HYDRO"/>
-      <sheetName val="Other_NUCL"/>
-      <sheetName val="Other_THERM"/>
-      <sheetName val="Other_CHP"/>
-      <sheetName val="Other_RENEW"/>
-      <sheetName val="Other_HEAT"/>
-      <sheetName val="ELC_FUELS"/>
-      <sheetName val="ELC"/>
-      <sheetName val="HEAT"/>
-      <sheetName val="CHP"/>
-      <sheetName val="ELC_EMI"/>
-      <sheetName val="Constant Table"/>
-      <sheetName val="ANS_ITEMS_DEL"/>
-      <sheetName val="ANS_ITEMS"/>
-      <sheetName val="ANS_TIDDATA"/>
-      <sheetName val="ANS_TSDATA"/>
-      <sheetName val="O&amp;M waste "/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>^FI_ST: TCH, PRC</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7494,7 +7380,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7823,17 +7709,17 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="21" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="60.33203125" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="9.1640625" style="21"/>
+    <col min="1" max="1" width="11.453125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="60.36328125" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="21"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="13">
       <c r="A3" s="20" t="s">
         <v>11</v>
       </c>
@@ -7884,20 +7770,20 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="25"/>
+    <col min="1" max="1" width="9.1796875" style="25"/>
     <col min="2" max="2" width="24" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="138.5" style="25" customWidth="1"/>
-    <col min="4" max="16384" width="9.1640625" style="25"/>
+    <col min="3" max="3" width="138.453125" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="19">
+    <row r="1" spans="2:3" ht="18.5">
       <c r="B1" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15">
+    <row r="3" spans="2:3" ht="14.5">
       <c r="B3" s="26" t="s">
         <v>16</v>
       </c>
@@ -7905,38 +7791,38 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15">
+    <row r="4" spans="2:3" ht="14.5">
       <c r="B4" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15">
+    <row r="5" spans="2:3" ht="14.5">
       <c r="B5" s="26"/>
     </row>
-    <row r="6" spans="2:3" ht="15">
+    <row r="6" spans="2:3" ht="14.5">
       <c r="B6" s="26"/>
     </row>
-    <row r="7" spans="2:3" ht="15">
+    <row r="7" spans="2:3" ht="14.5">
       <c r="B7" s="26"/>
     </row>
-    <row r="8" spans="2:3" ht="15">
+    <row r="8" spans="2:3" ht="14.5">
       <c r="B8" s="26"/>
     </row>
-    <row r="9" spans="2:3" ht="15">
+    <row r="9" spans="2:3" ht="14.5">
       <c r="B9" s="26"/>
     </row>
-    <row r="10" spans="2:3" ht="15">
+    <row r="10" spans="2:3" ht="14.5">
       <c r="B10" s="26"/>
     </row>
-    <row r="11" spans="2:3" ht="15">
+    <row r="11" spans="2:3" ht="14.5">
       <c r="B11" s="27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15">
+    <row r="12" spans="2:3" ht="14.5">
       <c r="B12" s="26"/>
     </row>
-    <row r="13" spans="2:3" ht="15">
+    <row r="13" spans="2:3" ht="14.5">
       <c r="B13" s="28" t="s">
         <v>19</v>
       </c>
@@ -7963,37 +7849,39 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:M29"/>
+  <dimension ref="B1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="2" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
-    <col min="7" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="12.453125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13">
+    <row r="1" spans="2:15">
       <c r="E1" s="14"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:15">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="2:13" ht="16" thickBot="1">
+    <row r="5" spans="2:15" ht="15" thickBot="1">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -8015,12 +7903,18 @@
       <c r="H5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="2:13" ht="16" thickBot="1">
+    <row r="6" spans="2:15" ht="15" thickBot="1">
       <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
@@ -8036,10 +7930,16 @@
       <c r="H6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="11"/>
+      <c r="I6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:15">
       <c r="B7" s="12"/>
       <c r="C7" s="13" t="s">
         <v>8</v>
@@ -8051,22 +7951,29 @@
         <v>2010</v>
       </c>
       <c r="F7" s="16">
+        <f>SUM(G7:J7)</f>
+        <v>40</v>
+      </c>
+      <c r="G7" s="16">
         <v>10</v>
       </c>
-      <c r="G7" s="16">
-        <f>F7*0.1</f>
-        <v>1</v>
-      </c>
       <c r="H7" s="16">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="I7" s="16">
+        <v>10</v>
+      </c>
+      <c r="J7" s="16">
         <f>G7</f>
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:15">
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
@@ -8077,22 +7984,30 @@
         <v>2012</v>
       </c>
       <c r="F8" s="16">
+        <f t="shared" ref="F8:F21" si="0">SUM(G8:J8)</f>
+        <v>40</v>
+      </c>
+      <c r="G8" s="16">
         <v>10</v>
-      </c>
-      <c r="G8" s="16">
-        <f>F8*0.1</f>
-        <v>1</v>
       </c>
       <c r="H8" s="16">
         <f>G8</f>
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="16">
+        <f>G8</f>
+        <v>10</v>
+      </c>
+      <c r="J8" s="16">
+        <f>G8</f>
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:15">
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -8103,21 +8018,29 @@
         <v>2020</v>
       </c>
       <c r="F9" s="16">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G9" s="16">
         <v>10</v>
       </c>
-      <c r="G9" s="16">
-        <f>F9*0.1</f>
-        <v>1</v>
-      </c>
       <c r="H9" s="16">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="I9" s="16">
         <f>G9</f>
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="16">
+        <f>G9</f>
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:15">
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
         <v>8</v>
@@ -8128,22 +8051,30 @@
       <c r="E10" s="9">
         <v>2030</v>
       </c>
-      <c r="F10" s="18">
-        <v>2223</v>
+      <c r="F10" s="16">
+        <f t="shared" si="0"/>
+        <v>889.2</v>
       </c>
       <c r="G10" s="16">
-        <f>F10*0.1</f>
         <v>222.3</v>
       </c>
       <c r="H10" s="16">
         <f>G10</f>
         <v>222.3</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="16">
+        <f>G10</f>
+        <v>222.3</v>
+      </c>
+      <c r="J10" s="16">
+        <f>G10</f>
+        <v>222.3</v>
+      </c>
+      <c r="K10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:15">
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -8154,9 +8085,9 @@
       <c r="E11" s="3">
         <v>2050</v>
       </c>
-      <c r="F11" s="17">
-        <f>F10*2</f>
-        <v>4446</v>
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>1778.4</v>
       </c>
       <c r="G11" s="17">
         <f>G10*2</f>
@@ -8166,15 +8097,23 @@
         <f>H10*2</f>
         <v>444.6</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="17">
+        <f>I10*2</f>
+        <v>444.6</v>
+      </c>
+      <c r="J11" s="17">
+        <f>J10*2</f>
+        <v>444.6</v>
+      </c>
+      <c r="K11" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="33" t="s">
+      <c r="N11" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="M11" s="33"/>
+      <c r="O11" s="33"/>
     </row>
-    <row r="12" spans="2:13">
+    <row r="12" spans="2:15">
       <c r="B12" s="9"/>
       <c r="C12" s="9" t="s">
         <v>8</v>
@@ -8185,23 +8124,31 @@
       <c r="E12" s="9">
         <v>2010</v>
       </c>
-      <c r="F12" s="18">
-        <f t="shared" ref="F12:H14" si="0">F7/2</f>
+      <c r="F12" s="16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" ref="F12:J14" si="1">G7/2</f>
         <v>5</v>
       </c>
-      <c r="G12" s="18">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
       <c r="H12" s="18">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="I12" s="10" t="s">
+        <f t="shared" ref="H12:I12" si="2">H7/2</f>
+        <v>5</v>
+      </c>
+      <c r="I12" s="18">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J12" s="18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:15">
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
         <v>8</v>
@@ -8212,23 +8159,31 @@
       <c r="E13" s="9">
         <v>2012</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G13" s="18">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
       <c r="H13" s="18">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="I13" s="10" t="s">
+        <f t="shared" ref="H13:I13" si="3">H8/2</f>
+        <v>5</v>
+      </c>
+      <c r="I13" s="18">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J13" s="18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:13">
+    <row r="14" spans="2:15">
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
         <v>8</v>
@@ -8239,23 +8194,31 @@
       <c r="E14" s="9">
         <v>2020</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="16">
         <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G14" s="18">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
       <c r="H14" s="18">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="I14" s="10" t="s">
+        <f t="shared" ref="H14:I14" si="4">H9/2</f>
+        <v>5</v>
+      </c>
+      <c r="I14" s="18">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="J14" s="18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:15">
       <c r="B15" s="9"/>
       <c r="C15" s="9" t="s">
         <v>8</v>
@@ -8266,23 +8229,31 @@
       <c r="E15" s="9">
         <v>2030</v>
       </c>
-      <c r="F15" s="18">
-        <f t="shared" ref="F15:H16" si="1">F10/2</f>
-        <v>1111.5</v>
+      <c r="F15" s="16">
+        <f t="shared" si="0"/>
+        <v>444.6</v>
       </c>
       <c r="G15" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F15:J16" si="5">G10/2</f>
         <v>111.15</v>
       </c>
       <c r="H15" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H15:I15" si="6">H10/2</f>
         <v>111.15</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="18">
+        <f t="shared" si="6"/>
+        <v>111.15</v>
+      </c>
+      <c r="J15" s="18">
+        <f t="shared" si="5"/>
+        <v>111.15</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:13">
+    <row r="16" spans="2:15">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>8</v>
@@ -8293,26 +8264,34 @@
       <c r="E16" s="3">
         <v>2040</v>
       </c>
-      <c r="F16" s="17">
-        <f t="shared" si="1"/>
-        <v>2223</v>
+      <c r="F16" s="16">
+        <f t="shared" si="0"/>
+        <v>889.2</v>
       </c>
       <c r="G16" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>222.3</v>
       </c>
       <c r="H16" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H16:I16" si="7">H11/2</f>
         <v>222.3</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="17">
+        <f t="shared" si="7"/>
+        <v>222.3</v>
+      </c>
+      <c r="J16" s="17">
+        <f t="shared" si="5"/>
+        <v>222.3</v>
+      </c>
+      <c r="K16" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="N16" s="33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:14">
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
         <v>8</v>
@@ -8323,23 +8302,31 @@
       <c r="E17" s="9">
         <v>2010</v>
       </c>
-      <c r="F17" s="18">
-        <f>F12/2</f>
-        <v>2.5</v>
+      <c r="F17" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="G17" s="18">
         <f>G12/2</f>
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
       <c r="H17" s="18">
         <f>H12/2</f>
-        <v>0.25</v>
-      </c>
-      <c r="I17" s="10" t="s">
+        <v>2.5</v>
+      </c>
+      <c r="I17" s="18">
+        <f>I12/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="J17" s="18">
+        <f>J12/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:14">
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
         <v>8</v>
@@ -8350,23 +8337,31 @@
       <c r="E18" s="9">
         <v>2012</v>
       </c>
-      <c r="F18" s="18">
-        <f t="shared" ref="F18:H18" si="2">F13/2</f>
+      <c r="F18" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="18">
+        <f t="shared" ref="F18:J18" si="8">G13/2</f>
         <v>2.5</v>
       </c>
-      <c r="G18" s="18">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
       <c r="H18" s="18">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="I18" s="10" t="s">
+        <f t="shared" ref="H18:I18" si="9">H13/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" si="9"/>
+        <v>2.5</v>
+      </c>
+      <c r="J18" s="18">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:14">
       <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
@@ -8376,23 +8371,31 @@
       <c r="E19" s="1">
         <v>2020</v>
       </c>
-      <c r="F19" s="18">
-        <f t="shared" ref="F19:H19" si="3">F14/2</f>
+      <c r="F19" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G19" s="18">
+        <f t="shared" ref="F19:J19" si="10">G14/2</f>
         <v>2.5</v>
       </c>
-      <c r="G19" s="18">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
       <c r="H19" s="18">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="I19" t="s">
+        <f t="shared" ref="H19:I19" si="11">H14/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" si="11"/>
+        <v>2.5</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="10"/>
+        <v>2.5</v>
+      </c>
+      <c r="K19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:14">
       <c r="C20" s="9" t="s">
         <v>8</v>
       </c>
@@ -8402,23 +8405,31 @@
       <c r="E20" s="9">
         <v>2030</v>
       </c>
-      <c r="F20" s="18">
-        <f t="shared" ref="F20:H20" si="4">F15/2</f>
-        <v>555.75</v>
+      <c r="F20" s="16">
+        <f t="shared" si="0"/>
+        <v>222.3</v>
       </c>
       <c r="G20" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F20:J20" si="12">G15/2</f>
         <v>55.575000000000003</v>
       </c>
       <c r="H20" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H20:I20" si="13">H15/2</f>
         <v>55.575000000000003</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="18">
+        <f t="shared" si="13"/>
+        <v>55.575000000000003</v>
+      </c>
+      <c r="J20" s="18">
+        <f t="shared" si="12"/>
+        <v>55.575000000000003</v>
+      </c>
+      <c r="K20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="16" thickBot="1">
+    <row r="21" spans="2:14" ht="15" thickBot="1">
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
@@ -8428,26 +8439,34 @@
       <c r="E21" s="3">
         <v>2040</v>
       </c>
-      <c r="F21" s="18">
-        <f t="shared" ref="F21:H21" si="5">F16/2</f>
-        <v>1111.5</v>
+      <c r="F21" s="16">
+        <f t="shared" si="0"/>
+        <v>444.6</v>
       </c>
       <c r="G21" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F21:J21" si="14">G16/2</f>
         <v>111.15</v>
       </c>
       <c r="H21" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H21:I21" si="15">H16/2</f>
         <v>111.15</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="18">
+        <f t="shared" si="15"/>
+        <v>111.15</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" si="14"/>
+        <v>111.15</v>
+      </c>
+      <c r="K21" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="33" t="s">
+      <c r="N21" s="33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:14">
       <c r="B22" s="30"/>
       <c r="C22" s="31" t="s">
         <v>8</v>
@@ -8467,20 +8486,27 @@
       <c r="H22" s="30">
         <v>5</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="30">
+        <v>5</v>
+      </c>
+      <c r="J22" s="30">
+        <v>5</v>
+      </c>
+      <c r="K22" s="32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
-      <c r="I27"/>
+    <row r="27" spans="2:14">
+      <c r="K27"/>
     </row>
-    <row r="28" spans="2:12">
-      <c r="I28"/>
+    <row r="28" spans="2:14">
+      <c r="K28"/>
     </row>
-    <row r="29" spans="2:12">
-      <c r="I29"/>
+    <row r="29" spans="2:14">
+      <c r="K29"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="77" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -8488,12 +8514,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8720,15 +8743,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29708D-970D-48DD-9E4A-5A0CFA626223}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3BDCBCB-54F4-4172-B29B-BA4C04015FBC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8753,10 +8780,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3BDCBCB-54F4-4172-B29B-BA4C04015FBC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29708D-970D-48DD-9E4A-5A0CFA626223}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>